<commit_message>
Fix 'rp' column to be more general -> Power_WeightsRP v0.1.1
</commit_message>
<xml_diff>
--- a/examples/Power_WeightsRP.xlsx
+++ b/examples/Power_WeightsRP.xlsx
@@ -611,7 +611,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Representative period for this hour</t>
+          <t>Representative period</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
@@ -963,7 +963,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Representative period for this hour</t>
+          <t>Representative period</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">

</xml_diff>